<commit_message>
fixed program and graph for all records
</commit_message>
<xml_diff>
--- a/GraphsMyUniqFixed.xlsx
+++ b/GraphsMyUniqFixed.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="16275" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="16275" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SCExon" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Chromosome</t>
   </si>
@@ -34,13 +34,25 @@
   <si>
     <t>Intron SL</t>
   </si>
+  <si>
+    <t>AVG:</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -71,14 +83,158 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -117,7 +273,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -139,155 +294,178 @@
             </c:strRef>
           </c:tx>
           <c:cat>
-            <c:numRef>
-              <c:f>Data!$A$2:$A$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+            <c:strRef>
+              <c:f>Data!$A$2:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>22</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="22">
+                  <c:v>X</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Y</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>M</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$22</c:f>
+              <c:f>Data!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>22454</c:v>
+                  <c:v>30944</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17645</c:v>
+                  <c:v>25085</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12916</c:v>
+                  <c:v>19217</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14563</c:v>
+                  <c:v>14029</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16061</c:v>
+                  <c:v>16042</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13861</c:v>
+                  <c:v>17627</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12022</c:v>
+                  <c:v>14967</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14647</c:v>
+                  <c:v>13078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11992</c:v>
+                  <c:v>15947</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14753</c:v>
+                  <c:v>13007</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15415</c:v>
+                  <c:v>16210</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7412</c:v>
+                  <c:v>16877</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9519</c:v>
+                  <c:v>8138</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10084</c:v>
+                  <c:v>10416</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11947</c:v>
+                  <c:v>11287</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14692</c:v>
+                  <c:v>13275</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5886</c:v>
+                  <c:v>16314</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16106</c:v>
+                  <c:v>6287</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7824</c:v>
+                  <c:v>17595</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5051</c:v>
+                  <c:v>8378</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6500</c:v>
+                  <c:v>5708</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7246</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12749</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1501</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="48898048"/>
-        <c:axId val="67243392"/>
+        <c:axId val="74028928"/>
+        <c:axId val="74044544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48898048"/>
+        <c:axId val="74028928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -308,18 +486,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67243392"/>
+        <c:crossAx val="74044544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67243392"/>
+        <c:axId val="74044544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -346,11 +523,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48898048"/>
+        <c:crossAx val="74028928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2500"/>
@@ -390,7 +566,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -412,155 +587,178 @@
             </c:strRef>
           </c:tx>
           <c:cat>
-            <c:numRef>
-              <c:f>Data!$A$2:$A$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+            <c:strRef>
+              <c:f>Data!$A$2:$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>22</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="22">
+                  <c:v>X</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Y</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>M</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$D$2:$D$22</c:f>
+              <c:f>Data!$D$2:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>46343.375</c:v>
+                  <c:v>64070.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36149.375</c:v>
+                  <c:v>51784.375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26963.625</c:v>
+                  <c:v>39423.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30131.875</c:v>
+                  <c:v>29272.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32859.625</c:v>
+                  <c:v>33233.625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28822.125</c:v>
+                  <c:v>36102.875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24837.625</c:v>
+                  <c:v>31148.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30507.25</c:v>
+                  <c:v>27000.625</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24648.25</c:v>
+                  <c:v>33214</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29878.75</c:v>
+                  <c:v>26686.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31528</c:v>
+                  <c:v>32842.75</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15490.625</c:v>
+                  <c:v>34557.25</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19572.375</c:v>
+                  <c:v>17098.875</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20585.125</c:v>
+                  <c:v>21368.375</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>24366.375</c:v>
+                  <c:v>23058.25</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29953.25</c:v>
+                  <c:v>27124.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>12206.375</c:v>
+                  <c:v>33201.75</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>33045.25</c:v>
+                  <c:v>13063.25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16058.375</c:v>
+                  <c:v>36036.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10624.625</c:v>
+                  <c:v>17212.375</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13415.625</c:v>
+                  <c:v>12043.25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14908.625</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>26472.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3210.875</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>55.875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="48899968"/>
-        <c:axId val="102720256"/>
+        <c:axId val="67925120"/>
+        <c:axId val="67927040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48899968"/>
+        <c:axId val="67925120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -581,18 +779,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102720256"/>
+        <c:crossAx val="67927040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102720256"/>
+        <c:axId val="67927040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -614,11 +811,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48899968"/>
+        <c:crossAx val="67925120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -632,7 +828,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="78" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -989,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1020,236 +1216,299 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>22454</v>
+        <v>30944</v>
       </c>
       <c r="D2" s="1">
-        <v>46343.375</v>
+        <v>64070.75</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>17645</v>
+        <v>25085</v>
       </c>
       <c r="D3" s="1">
-        <v>36149.375</v>
+        <v>51784.375</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>12916</v>
+        <v>19217</v>
       </c>
       <c r="D4" s="1">
-        <v>26963.625</v>
+        <v>39423.5</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>14563</v>
+        <v>14029</v>
       </c>
       <c r="D5" s="1">
-        <v>30131.875</v>
+        <v>29272.75</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>16061</v>
+        <v>16042</v>
       </c>
       <c r="D6" s="1">
-        <v>32859.625</v>
+        <v>33233.625</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>13861</v>
+        <v>17627</v>
       </c>
       <c r="D7" s="1">
-        <v>28822.125</v>
+        <v>36102.875</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>12022</v>
+        <v>14967</v>
       </c>
       <c r="D8" s="1">
-        <v>24837.625</v>
+        <v>31148.75</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>14647</v>
+        <v>13078</v>
       </c>
       <c r="D9" s="1">
-        <v>30507.25</v>
+        <v>27000.625</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>11992</v>
+        <v>15947</v>
       </c>
       <c r="D10" s="1">
-        <v>24648.25</v>
+        <v>33214</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>14753</v>
+        <v>13007</v>
       </c>
       <c r="D11" s="1">
-        <v>29878.75</v>
+        <v>26686.75</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>15415</v>
+        <v>16210</v>
       </c>
       <c r="D12" s="1">
-        <v>31528</v>
+        <v>32842.75</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>7412</v>
+        <v>16877</v>
       </c>
       <c r="D13" s="1">
-        <v>15490.625</v>
+        <v>34557.25</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>9519</v>
+        <v>8138</v>
       </c>
       <c r="D14" s="1">
-        <v>19572.375</v>
+        <v>17098.875</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>10084</v>
+        <v>10416</v>
       </c>
       <c r="D15" s="1">
-        <v>20585.125</v>
+        <v>21368.375</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>11947</v>
+        <v>11287</v>
       </c>
       <c r="D16" s="1">
-        <v>24366.375</v>
+        <v>23058.25</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>14692</v>
+        <v>13275</v>
       </c>
       <c r="D17" s="1">
-        <v>29953.25</v>
+        <v>27124.75</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>5886</v>
+        <v>16314</v>
       </c>
       <c r="D18" s="1">
-        <v>12206.375</v>
+        <v>33201.75</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>16106</v>
+        <v>6287</v>
       </c>
       <c r="D19" s="1">
-        <v>33045.25</v>
+        <v>13063.25</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>7824</v>
+        <v>17595</v>
       </c>
       <c r="D20" s="1">
-        <v>16058.375</v>
+        <v>36036.5</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>5051</v>
+        <v>8378</v>
       </c>
       <c r="D21" s="1">
-        <v>10624.625</v>
+        <v>17212.375</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>5708</v>
+      </c>
+      <c r="D22" s="1">
+        <v>12043.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B22">
-        <v>6500</v>
-      </c>
-      <c r="D22" s="1">
-        <v>13415.625</v>
+      <c r="B23">
+        <v>7246</v>
+      </c>
+      <c r="D23" s="1">
+        <v>14908.625</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>12749</v>
+      </c>
+      <c r="D24" s="1">
+        <v>26472.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>1501</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3210.875</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>31</v>
+      </c>
+      <c r="D26" s="1">
+        <v>55.875</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <f>AVERAGE(B2:B26)</f>
+        <v>13278.2</v>
+      </c>
+      <c r="D28" s="1">
+        <f>AVERAGE(D2:D26)</f>
+        <v>27367.73</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B26">
+    <cfRule type="aboveAverage" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D26">
+    <cfRule type="aboveAverage" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>